<commit_message>
updated codebook to v5
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D30240-F6C8-4C48-B7DB-D15A5488B6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B77789-C8DE-834B-B216-163D37E9EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="542">
   <si>
     <t>Nr</t>
   </si>
@@ -1645,7 +1645,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>TODO TE variable kreieren</t>
+    <t>no carework//carework</t>
   </si>
 </sst>
 </file>
@@ -2006,11 +2006,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G384" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="K99" sqref="J99:K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2774,7 +2774,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -3063,12 +3063,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>41.5</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>537</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>541</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>509</v>
@@ -3079,11 +3085,8 @@
       <c r="M44" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="N44" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -4761,12 +4764,6 @@
       <c r="I99" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="J99" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="K99" s="2" t="s">
-        <v>522</v>
-      </c>
     </row>
     <row r="100" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
@@ -5875,7 +5872,7 @@
         <v>524</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N135" s="2" t="s">
         <v>529</v>
@@ -5910,7 +5907,7 @@
         <v>524</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="137" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5942,7 +5939,7 @@
         <v>524</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5974,7 +5971,7 @@
         <v>524</v>
       </c>
       <c r="K138" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6006,7 +6003,7 @@
         <v>524</v>
       </c>
       <c r="K139" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6038,7 +6035,7 @@
         <v>524</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6070,7 +6067,7 @@
         <v>524</v>
       </c>
       <c r="K141" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6102,7 +6099,7 @@
         <v>524</v>
       </c>
       <c r="K142" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="143" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6134,7 +6131,7 @@
         <v>524</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="144" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6166,7 +6163,7 @@
         <v>524</v>
       </c>
       <c r="K144" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="145" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6198,7 +6195,7 @@
         <v>525</v>
       </c>
       <c r="K145" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6230,7 +6227,7 @@
         <v>525</v>
       </c>
       <c r="K146" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="147" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6262,7 +6259,7 @@
         <v>525</v>
       </c>
       <c r="K147" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6294,7 +6291,7 @@
         <v>525</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6326,7 +6323,7 @@
         <v>526</v>
       </c>
       <c r="K149" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6358,7 +6355,7 @@
         <v>526</v>
       </c>
       <c r="K150" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6390,7 +6387,7 @@
         <v>526</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6422,7 +6419,7 @@
         <v>526</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6454,7 +6451,7 @@
         <v>527</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6486,7 +6483,7 @@
         <v>527</v>
       </c>
       <c r="K154" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6518,7 +6515,7 @@
         <v>527</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="156" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6550,7 +6547,7 @@
         <v>527</v>
       </c>
       <c r="K156" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="157" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6582,7 +6579,7 @@
         <v>528</v>
       </c>
       <c r="K157" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="158" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -6614,7 +6611,7 @@
         <v>528</v>
       </c>
       <c r="K158" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="159" spans="1:11" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
zk update title for multibar and color scheme
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkovacevic\Desktop\Ehrenamt\Actionuni\SWiMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B91941-2859-4FA2-AEEF-E70A7D228FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B77789-C8DE-834B-B216-163D37E9EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2007,29 +2007,29 @@
   <dimension ref="A1:N225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J66" sqref="J66"/>
+      <selection pane="bottomRight" activeCell="K99" sqref="J99:K99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2"/>
-    <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="7" width="48.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="18.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="52.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="48.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
     <col min="9" max="9" width="47" style="2" customWidth="1"/>
-    <col min="10" max="13" width="12.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="39.140625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="10.85546875" style="2"/>
+    <col min="10" max="13" width="12.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="39.1640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22.5</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>41.5</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>46</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>47</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>48</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>49</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>50</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>51</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>52</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>53</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>54</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>55</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>56</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>57</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>58</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>59</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>60</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>61</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>62</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>63</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>64</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>65</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>66</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>67</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>68</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>69</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>70</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>71</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>72</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>73</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>74</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>75</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>76</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>77</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>78</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>79</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>80</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>81</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>82</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>83</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>84</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>85</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>86</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>87</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>88</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>89</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>90</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>91</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>92</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>93</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>94</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>95</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>96</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>97</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>98</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>99</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>100</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>101</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>102</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>103</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>104</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>105</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>106</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>107</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>108</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>109</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>110</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>111</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>112</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>113</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>114</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>115</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>116</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>117</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>118</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>119</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>120</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>121</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>122</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>123</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>124</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>125</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>126</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>127</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>128</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>129</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>130</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>131</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>132</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>133</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>134</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>135</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>136</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>137</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>138</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>139</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>140</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>141</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>142</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>143</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>144</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>145</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>146</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>147</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>148</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>149</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>150</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>151</v>
       </c>
@@ -6486,7 +6486,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>152</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>153</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>154</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>155</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>156</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>157</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>158</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>159</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>160</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>161</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>162</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>163</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>164</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>165</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>165.5</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>166</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>167</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>168</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>169</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>170</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>171</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>172</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>173</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>174</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>175</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>176</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>177</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>178</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>179</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>180</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>181</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>182</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>183</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>184</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>185</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>186</v>
       </c>
@@ -7332,7 +7332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>187</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>188</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>189</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>190</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>191</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>192</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>193</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>194</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>195</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>196</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>197</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>198</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>199</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>200</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>201</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>202</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
         <v>203</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>204</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>205</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>206</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>207</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>208</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>209</v>
       </c>
@@ -7705,7 +7705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>210</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>211</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>212</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>213</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>214</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>215</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>216</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>217</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>218</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>219</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>220</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
collected todos, established structure, fontSize argument
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B77789-C8DE-834B-B216-163D37E9EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364BCF8D-62B3-DD49-90E1-4527E091BA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="-8660" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="542">
   <si>
     <t>Nr</t>
   </si>
@@ -2006,11 +2018,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K99" sqref="J99:K99"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2338,6 +2350,9 @@
       <c r="J17" s="2" t="s">
         <v>509</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -2355,9 +2370,6 @@
       <c r="E18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>509</v>
-      </c>
     </row>
     <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -2387,6 +2399,9 @@
       <c r="J19" s="2" t="s">
         <v>509</v>
       </c>
+      <c r="K19" s="2" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -2549,6 +2564,9 @@
       <c r="L25" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="M25" s="2" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -2610,12 +2628,6 @@
       <c r="I27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="28" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -2642,12 +2654,6 @@
       <c r="I28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="29" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -2662,12 +2668,6 @@
       <c r="D29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="30" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -2694,12 +2694,6 @@
       <c r="I30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="31" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -2789,12 +2783,6 @@
       </c>
       <c r="E33" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update function and insitiuional report
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkovacevic\Desktop\Ehrenamt\Actionuni\SWiMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89632F23-E5A6-E646-975D-97C903F4D986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3A153-7EA4-48AE-BB38-AE96421BE297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-8600" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1743,15 +1743,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2064,29 +2061,29 @@
   <dimension ref="A1:N232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.85546875" style="2"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="52.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="48.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="18.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2"/>
+    <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2"/>
+    <col min="7" max="7" width="48.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="2"/>
     <col min="9" max="9" width="47" style="2" customWidth="1"/>
-    <col min="10" max="13" width="12.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="39.1640625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="2"/>
+    <col min="10" max="13" width="12.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2141,7 +2138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2155,7 +2152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2169,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2183,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2197,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2211,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2225,7 +2222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2239,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2267,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2281,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2321,7 +2318,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2344,7 +2341,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2367,7 +2364,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2399,7 +2396,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2416,7 +2413,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2448,7 +2445,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18.5</v>
       </c>
@@ -2471,7 +2468,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2497,7 +2494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2549,7 +2546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2575,7 +2572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22.5</v>
       </c>
@@ -2601,7 +2598,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2633,7 +2630,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23.5</v>
       </c>
@@ -2653,7 +2650,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2685,7 +2682,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>24.5</v>
       </c>
@@ -2702,7 +2699,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>25</v>
       </c>
@@ -2728,7 +2725,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>26</v>
       </c>
@@ -2754,7 +2751,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>27</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>28</v>
       </c>
@@ -2794,7 +2791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>29</v>
       </c>
@@ -2826,7 +2823,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>29.5</v>
       </c>
@@ -2846,7 +2843,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>30</v>
       </c>
@@ -2878,7 +2875,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>30.5</v>
       </c>
@@ -2895,7 +2892,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>31</v>
       </c>
@@ -2912,7 +2909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>32</v>
       </c>
@@ -2944,7 +2941,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>33</v>
       </c>
@@ -2976,7 +2973,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>34</v>
       </c>
@@ -3002,7 +2999,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>35</v>
       </c>
@@ -3022,7 +3019,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>36</v>
       </c>
@@ -3042,7 +3039,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>37</v>
       </c>
@@ -3074,7 +3071,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>38</v>
       </c>
@@ -3100,7 +3097,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>39</v>
       </c>
@@ -3126,7 +3123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>40</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>41</v>
       </c>
@@ -3178,11 +3175,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>41.5</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>546</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -3198,7 +3195,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>42</v>
       </c>
@@ -3224,7 +3221,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43</v>
       </c>
@@ -3250,7 +3247,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44</v>
       </c>
@@ -3276,7 +3273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45</v>
       </c>
@@ -3302,7 +3299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>46</v>
       </c>
@@ -3328,7 +3325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -3354,7 +3351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>48</v>
       </c>
@@ -3380,7 +3377,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>49</v>
       </c>
@@ -3406,7 +3403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>50</v>
       </c>
@@ -3432,7 +3429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>51</v>
       </c>
@@ -3449,7 +3446,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>52</v>
       </c>
@@ -3481,7 +3478,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>53</v>
       </c>
@@ -3513,7 +3510,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>54</v>
       </c>
@@ -3545,7 +3542,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>55</v>
       </c>
@@ -3577,7 +3574,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>56</v>
       </c>
@@ -3609,7 +3606,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>57</v>
       </c>
@@ -3641,7 +3638,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>58</v>
       </c>
@@ -3673,7 +3670,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>59</v>
       </c>
@@ -3705,7 +3702,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>60</v>
       </c>
@@ -3737,7 +3734,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>61</v>
       </c>
@@ -3769,7 +3766,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>62</v>
       </c>
@@ -3801,7 +3798,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>63</v>
       </c>
@@ -3833,7 +3830,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>64</v>
       </c>
@@ -3865,7 +3862,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>65</v>
       </c>
@@ -3897,7 +3894,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>66</v>
       </c>
@@ -3929,7 +3926,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>67</v>
       </c>
@@ -3961,7 +3958,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>68</v>
       </c>
@@ -3993,7 +3990,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>69</v>
       </c>
@@ -4019,7 +4016,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>70</v>
       </c>
@@ -4051,7 +4048,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>71</v>
       </c>
@@ -4083,7 +4080,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>72</v>
       </c>
@@ -4115,7 +4112,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>73</v>
       </c>
@@ -4147,7 +4144,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>74</v>
       </c>
@@ -4179,7 +4176,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>75</v>
       </c>
@@ -4211,7 +4208,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>76</v>
       </c>
@@ -4243,7 +4240,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>77</v>
       </c>
@@ -4275,7 +4272,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>78</v>
       </c>
@@ -4307,7 +4304,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>79</v>
       </c>
@@ -4339,7 +4336,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>80</v>
       </c>
@@ -4371,7 +4368,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>81</v>
       </c>
@@ -4403,7 +4400,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>82</v>
       </c>
@@ -4435,7 +4432,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>83</v>
       </c>
@@ -4467,7 +4464,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>84</v>
       </c>
@@ -4499,7 +4496,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>85</v>
       </c>
@@ -4531,7 +4528,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>86</v>
       </c>
@@ -4563,7 +4560,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>87</v>
       </c>
@@ -4595,7 +4592,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>88</v>
       </c>
@@ -4627,7 +4624,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>89</v>
       </c>
@@ -4659,7 +4656,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>90</v>
       </c>
@@ -4691,7 +4688,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>91</v>
       </c>
@@ -4723,7 +4720,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>92</v>
       </c>
@@ -4755,7 +4752,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>93</v>
       </c>
@@ -4787,7 +4784,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>94</v>
       </c>
@@ -4819,7 +4816,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>95</v>
       </c>
@@ -4851,7 +4848,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>96</v>
       </c>
@@ -4877,7 +4874,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>97</v>
       </c>
@@ -4909,7 +4906,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>98</v>
       </c>
@@ -4935,7 +4932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>99</v>
       </c>
@@ -4961,7 +4958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>100</v>
       </c>
@@ -4987,7 +4984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>101</v>
       </c>
@@ -5013,7 +5010,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>102</v>
       </c>
@@ -5039,7 +5036,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>103</v>
       </c>
@@ -5065,7 +5062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>104</v>
       </c>
@@ -5091,7 +5088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>105</v>
       </c>
@@ -5123,7 +5120,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>106</v>
       </c>
@@ -5155,7 +5152,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>107</v>
       </c>
@@ -5187,7 +5184,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>108</v>
       </c>
@@ -5219,7 +5216,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>109</v>
       </c>
@@ -5251,7 +5248,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>110</v>
       </c>
@@ -5283,7 +5280,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>111</v>
       </c>
@@ -5315,7 +5312,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>112</v>
       </c>
@@ -5347,7 +5344,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>113</v>
       </c>
@@ -5379,7 +5376,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>114</v>
       </c>
@@ -5411,7 +5408,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>115</v>
       </c>
@@ -5443,7 +5440,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>116</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>117</v>
       </c>
@@ -5507,7 +5504,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>118</v>
       </c>
@@ -5539,7 +5536,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>119</v>
       </c>
@@ -5571,7 +5568,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>120</v>
       </c>
@@ -5603,7 +5600,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>121</v>
       </c>
@@ -5635,7 +5632,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>122</v>
       </c>
@@ -5667,7 +5664,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>123</v>
       </c>
@@ -5699,7 +5696,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>124</v>
       </c>
@@ -5731,7 +5728,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>125</v>
       </c>
@@ -5763,7 +5760,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>126</v>
       </c>
@@ -5795,7 +5792,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>127</v>
       </c>
@@ -5827,7 +5824,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>128</v>
       </c>
@@ -5859,7 +5856,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>129</v>
       </c>
@@ -5891,7 +5888,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>130</v>
       </c>
@@ -5923,7 +5920,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>131</v>
       </c>
@@ -5955,7 +5952,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>132</v>
       </c>
@@ -5990,7 +5987,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>133</v>
       </c>
@@ -6022,7 +6019,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>134</v>
       </c>
@@ -6054,7 +6051,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>135</v>
       </c>
@@ -6086,7 +6083,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>136</v>
       </c>
@@ -6118,7 +6115,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>137</v>
       </c>
@@ -6150,7 +6147,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>138</v>
       </c>
@@ -6182,7 +6179,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>139</v>
       </c>
@@ -6214,7 +6211,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>140</v>
       </c>
@@ -6246,7 +6243,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>141</v>
       </c>
@@ -6278,7 +6275,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>142</v>
       </c>
@@ -6310,7 +6307,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>143</v>
       </c>
@@ -6342,7 +6339,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>144</v>
       </c>
@@ -6374,7 +6371,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>145</v>
       </c>
@@ -6406,7 +6403,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>146</v>
       </c>
@@ -6438,7 +6435,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>147</v>
       </c>
@@ -6470,7 +6467,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>148</v>
       </c>
@@ -6502,7 +6499,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>149</v>
       </c>
@@ -6534,7 +6531,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>150</v>
       </c>
@@ -6566,7 +6563,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>151</v>
       </c>
@@ -6598,7 +6595,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>152</v>
       </c>
@@ -6630,7 +6627,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>153</v>
       </c>
@@ -6662,7 +6659,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>154</v>
       </c>
@@ -6694,7 +6691,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>155</v>
       </c>
@@ -6726,7 +6723,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>156</v>
       </c>
@@ -6752,7 +6749,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>157</v>
       </c>
@@ -6772,7 +6769,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>158</v>
       </c>
@@ -6804,7 +6801,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>159</v>
       </c>
@@ -6839,7 +6836,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>160</v>
       </c>
@@ -6871,7 +6868,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>161</v>
       </c>
@@ -6903,7 +6900,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>162</v>
       </c>
@@ -6935,7 +6932,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>163</v>
       </c>
@@ -6967,7 +6964,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>164</v>
       </c>
@@ -6999,7 +6996,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>165</v>
       </c>
@@ -7031,7 +7028,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>165.5</v>
       </c>
@@ -7054,7 +7051,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>165.6</v>
       </c>
@@ -7065,7 +7062,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>166</v>
       </c>
@@ -7097,7 +7094,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>166.5</v>
       </c>
@@ -7129,7 +7126,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>167</v>
       </c>
@@ -7161,7 +7158,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>168</v>
       </c>
@@ -7193,7 +7190,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>169</v>
       </c>
@@ -7225,7 +7222,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>170</v>
       </c>
@@ -7251,7 +7248,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>171</v>
       </c>
@@ -7277,7 +7274,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>172</v>
       </c>
@@ -7291,7 +7288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>173</v>
       </c>
@@ -7305,7 +7302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>174</v>
       </c>
@@ -7319,7 +7316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>175</v>
       </c>
@@ -7333,7 +7330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>176</v>
       </c>
@@ -7347,7 +7344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>177</v>
       </c>
@@ -7361,7 +7358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>178</v>
       </c>
@@ -7375,7 +7372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>179</v>
       </c>
@@ -7389,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>180</v>
       </c>
@@ -7403,7 +7400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>181</v>
       </c>
@@ -7417,7 +7414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>182</v>
       </c>
@@ -7431,7 +7428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>183</v>
       </c>
@@ -7445,7 +7442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>184</v>
       </c>
@@ -7459,7 +7456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>185</v>
       </c>
@@ -7473,7 +7470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>186</v>
       </c>
@@ -7487,7 +7484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>187</v>
       </c>
@@ -7501,7 +7498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>188</v>
       </c>
@@ -7512,7 +7509,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>189</v>
       </c>
@@ -7523,7 +7520,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>190</v>
       </c>
@@ -7537,7 +7534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>191</v>
       </c>
@@ -7554,7 +7551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>192</v>
       </c>
@@ -7571,7 +7568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>193</v>
       </c>
@@ -7588,7 +7585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>194</v>
       </c>
@@ -7605,7 +7602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>195</v>
       </c>
@@ -7622,7 +7619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>196</v>
       </c>
@@ -7639,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>197</v>
       </c>
@@ -7656,7 +7653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>198</v>
       </c>
@@ -7673,7 +7670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>199</v>
       </c>
@@ -7690,7 +7687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>200</v>
       </c>
@@ -7707,7 +7704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>201</v>
       </c>
@@ -7724,7 +7721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>202</v>
       </c>
@@ -7741,7 +7738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>203</v>
       </c>
@@ -7758,7 +7755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>204</v>
       </c>
@@ -7775,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>205</v>
       </c>
@@ -7792,7 +7789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>206</v>
       </c>
@@ -7809,7 +7806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>207</v>
       </c>
@@ -7826,7 +7823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>208</v>
       </c>
@@ -7843,7 +7840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>209</v>
       </c>
@@ -7860,7 +7857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>210</v>
       </c>
@@ -7877,7 +7874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>211</v>
       </c>
@@ -7894,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>212</v>
       </c>
@@ -7911,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>213</v>
       </c>
@@ -7928,7 +7925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>214</v>
       </c>
@@ -7945,7 +7942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>215</v>
       </c>
@@ -7962,7 +7959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>216</v>
       </c>
@@ -7979,7 +7976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>217</v>
       </c>
@@ -7996,7 +7993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>218</v>
       </c>
@@ -8013,7 +8010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>219</v>
       </c>
@@ -8030,7 +8027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>220</v>
       </c>
@@ -8047,7 +8044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
aggregation plot without institution
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkovacevic\Desktop\Ehrenamt\Actionuni\SWiMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99879BBD-3B15-4AD9-A179-6F254DFC35A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EA05BC-E2D0-464C-8D37-1B369C7C10B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="557">
   <si>
     <t>Nr</t>
   </si>
@@ -1633,6 +1633,9 @@
     <t>from DASS scale</t>
   </si>
   <si>
+    <t>facet_wrap with items above</t>
+  </si>
+  <si>
     <t>burnout</t>
   </si>
   <si>
@@ -1699,7 +1702,7 @@
     <t>Researcher aiming for a PhD//Researcher with a PhD//Other</t>
   </si>
   <si>
-    <t>depression_sum</t>
+    <t>Other 2(please specify)</t>
   </si>
 </sst>
 </file>
@@ -1743,12 +1746,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2061,29 +2067,29 @@
   <dimension ref="A1:N232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B152" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J123" sqref="J123"/>
+      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2"/>
-    <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="2"/>
-    <col min="7" max="7" width="48.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="18.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="52.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="48.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
     <col min="9" max="9" width="47" style="2" customWidth="1"/>
-    <col min="10" max="13" width="12.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="39.140625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="10.85546875" style="2"/>
+    <col min="10" max="13" width="12.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="39.1640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2118,16 +2124,16 @@
         <v>519</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2138,7 +2144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2194,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2278,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2292,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2318,7 +2324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18.5</v>
       </c>
@@ -2453,22 +2459,22 @@
         <v>225</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>537</v>
-      </c>
       <c r="M20" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2572,18 +2578,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>22.5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>234</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>509</v>
@@ -2592,13 +2598,13 @@
         <v>510</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2630,27 +2636,27 @@
         <v>510</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>23.5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>537</v>
-      </c>
       <c r="M27" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2682,24 +2688,24 @@
         <v>510</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>24.5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>25</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>26</v>
       </c>
@@ -2751,7 +2757,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>27</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>28</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>29</v>
       </c>
@@ -2823,27 +2829,27 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>29.5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>537</v>
-      </c>
       <c r="M35" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>30</v>
       </c>
@@ -2875,24 +2881,24 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>30.5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="M37" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>31</v>
       </c>
@@ -2909,7 +2915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>32</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>33</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>34</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>35</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>36</v>
       </c>
@@ -3039,7 +3045,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>37</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>38</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>39</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>40</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>41</v>
       </c>
@@ -3175,27 +3181,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>41.5</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>545</v>
+      <c r="B49" s="3" t="s">
+        <v>546</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>509</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>42</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43</v>
       </c>
@@ -3247,7 +3253,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>45</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>46</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>48</v>
       </c>
@@ -3377,7 +3383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>49</v>
       </c>
@@ -3403,7 +3409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>50</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>51</v>
       </c>
@@ -3446,7 +3452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>52</v>
       </c>
@@ -3478,7 +3484,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>53</v>
       </c>
@@ -3510,7 +3516,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>54</v>
       </c>
@@ -3542,7 +3548,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>55</v>
       </c>
@@ -3574,7 +3580,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>56</v>
       </c>
@@ -3606,7 +3612,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>57</v>
       </c>
@@ -3638,7 +3644,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>58</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>59</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>60</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>61</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>62</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>63</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>64</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>65</v>
       </c>
@@ -3894,7 +3900,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>66</v>
       </c>
@@ -3926,7 +3932,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>67</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>68</v>
       </c>
@@ -3990,7 +3996,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>69</v>
       </c>
@@ -4016,7 +4022,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>70</v>
       </c>
@@ -4048,7 +4054,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>71</v>
       </c>
@@ -4080,7 +4086,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>72</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>73</v>
       </c>
@@ -4144,7 +4150,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>74</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>75</v>
       </c>
@@ -4208,7 +4214,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>76</v>
       </c>
@@ -4240,7 +4246,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>77</v>
       </c>
@@ -4272,7 +4278,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>78</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>79</v>
       </c>
@@ -4336,7 +4342,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>80</v>
       </c>
@@ -4368,7 +4374,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>81</v>
       </c>
@@ -4400,7 +4406,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>82</v>
       </c>
@@ -4432,7 +4438,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>83</v>
       </c>
@@ -4464,7 +4470,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>84</v>
       </c>
@@ -4496,7 +4502,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>85</v>
       </c>
@@ -4528,7 +4534,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>86</v>
       </c>
@@ -4560,7 +4566,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>87</v>
       </c>
@@ -4592,7 +4598,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>88</v>
       </c>
@@ -4624,7 +4630,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>89</v>
       </c>
@@ -4656,7 +4662,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>90</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>91</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>92</v>
       </c>
@@ -4752,7 +4758,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>93</v>
       </c>
@@ -4784,7 +4790,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>94</v>
       </c>
@@ -4816,7 +4822,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>95</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>96</v>
       </c>
@@ -4874,7 +4880,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>97</v>
       </c>
@@ -4899,8 +4905,14 @@
       <c r="I105" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="J105" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>98</v>
       </c>
@@ -4926,7 +4938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>99</v>
       </c>
@@ -4952,7 +4964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>100</v>
       </c>
@@ -4978,7 +4990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>101</v>
       </c>
@@ -5004,7 +5016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>102</v>
       </c>
@@ -5030,7 +5042,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>103</v>
       </c>
@@ -5056,7 +5068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>104</v>
       </c>
@@ -5082,7 +5094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>105</v>
       </c>
@@ -5114,7 +5126,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>106</v>
       </c>
@@ -5146,7 +5158,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>107</v>
       </c>
@@ -5178,7 +5190,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>108</v>
       </c>
@@ -5210,7 +5222,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>109</v>
       </c>
@@ -5242,7 +5254,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>110</v>
       </c>
@@ -5274,7 +5286,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>111</v>
       </c>
@@ -5306,7 +5318,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>112</v>
       </c>
@@ -5338,7 +5350,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>113</v>
       </c>
@@ -5370,7 +5382,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>114</v>
       </c>
@@ -5402,7 +5414,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>115</v>
       </c>
@@ -5434,7 +5446,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>116</v>
       </c>
@@ -5466,7 +5478,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>117</v>
       </c>
@@ -5498,7 +5510,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>118</v>
       </c>
@@ -5530,7 +5542,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>119</v>
       </c>
@@ -5562,7 +5574,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>120</v>
       </c>
@@ -5594,7 +5606,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>121</v>
       </c>
@@ -5626,7 +5638,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>122</v>
       </c>
@@ -5658,7 +5670,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>123</v>
       </c>
@@ -5690,7 +5702,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>124</v>
       </c>
@@ -5722,7 +5734,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>125</v>
       </c>
@@ -5754,7 +5766,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>126</v>
       </c>
@@ -5786,7 +5798,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>127</v>
       </c>
@@ -5818,7 +5830,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>128</v>
       </c>
@@ -5832,7 +5844,7 @@
         <v>38</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>254</v>
+        <v>556</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>301</v>
@@ -5843,8 +5855,14 @@
       <c r="I136" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="J136" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>129</v>
       </c>
@@ -5876,7 +5894,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>130</v>
       </c>
@@ -5908,7 +5926,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>131</v>
       </c>
@@ -5940,7 +5958,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>132</v>
       </c>
@@ -5975,7 +5993,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>133</v>
       </c>
@@ -6007,7 +6025,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>134</v>
       </c>
@@ -6039,7 +6057,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>135</v>
       </c>
@@ -6071,7 +6089,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>136</v>
       </c>
@@ -6103,7 +6121,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>137</v>
       </c>
@@ -6135,7 +6153,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>138</v>
       </c>
@@ -6167,7 +6185,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>139</v>
       </c>
@@ -6199,7 +6217,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>140</v>
       </c>
@@ -6231,7 +6249,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>141</v>
       </c>
@@ -6263,7 +6281,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>142</v>
       </c>
@@ -6295,7 +6313,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>143</v>
       </c>
@@ -6327,7 +6345,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>144</v>
       </c>
@@ -6359,7 +6377,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>145</v>
       </c>
@@ -6391,7 +6409,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>146</v>
       </c>
@@ -6423,7 +6441,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>147</v>
       </c>
@@ -6455,7 +6473,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>148</v>
       </c>
@@ -6487,7 +6505,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>149</v>
       </c>
@@ -6519,7 +6537,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>150</v>
       </c>
@@ -6551,7 +6569,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>151</v>
       </c>
@@ -6583,7 +6601,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>152</v>
       </c>
@@ -6615,7 +6633,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>153</v>
       </c>
@@ -6647,7 +6665,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>154</v>
       </c>
@@ -6679,7 +6697,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>155</v>
       </c>
@@ -6711,7 +6729,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>156</v>
       </c>
@@ -6737,7 +6755,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>157</v>
       </c>
@@ -6757,7 +6775,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>158</v>
       </c>
@@ -6789,7 +6807,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>159</v>
       </c>
@@ -6824,7 +6842,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>160</v>
       </c>
@@ -6856,7 +6874,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>161</v>
       </c>
@@ -6888,7 +6906,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>162</v>
       </c>
@@ -6920,7 +6938,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>163</v>
       </c>
@@ -6952,7 +6970,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>164</v>
       </c>
@@ -6984,7 +7002,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>165</v>
       </c>
@@ -7016,12 +7034,12 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>165.5</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>517</v>
@@ -7030,24 +7048,27 @@
         <v>518</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>555</v>
+        <v>516</v>
       </c>
       <c r="K174" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+      <c r="N174" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>165.6</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>166</v>
       </c>
@@ -7073,18 +7094,18 @@
         <v>408</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>166.5</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>405</v>
@@ -7105,13 +7126,13 @@
         <v>408</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="K177" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>167</v>
       </c>
@@ -7143,7 +7164,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>168</v>
       </c>
@@ -7169,13 +7190,13 @@
         <v>417</v>
       </c>
       <c r="J179" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="K179" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>169</v>
       </c>
@@ -7201,13 +7222,13 @@
         <v>417</v>
       </c>
       <c r="J180" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="K180" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>170</v>
       </c>
@@ -7233,7 +7254,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>171</v>
       </c>
@@ -7259,7 +7280,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>172</v>
       </c>
@@ -7273,7 +7294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>173</v>
       </c>
@@ -7287,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>174</v>
       </c>
@@ -7301,7 +7322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>175</v>
       </c>
@@ -7315,7 +7336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>176</v>
       </c>
@@ -7329,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>177</v>
       </c>
@@ -7343,7 +7364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>178</v>
       </c>
@@ -7357,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>179</v>
       </c>
@@ -7371,7 +7392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>180</v>
       </c>
@@ -7385,7 +7406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>181</v>
       </c>
@@ -7399,7 +7420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>182</v>
       </c>
@@ -7413,7 +7434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>183</v>
       </c>
@@ -7427,7 +7448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>184</v>
       </c>
@@ -7441,7 +7462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>185</v>
       </c>
@@ -7455,7 +7476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>186</v>
       </c>
@@ -7469,7 +7490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>187</v>
       </c>
@@ -7483,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>188</v>
       </c>
@@ -7494,7 +7515,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>189</v>
       </c>
@@ -7505,7 +7526,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>190</v>
       </c>
@@ -7519,7 +7540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>191</v>
       </c>
@@ -7536,7 +7557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>192</v>
       </c>
@@ -7553,7 +7574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>193</v>
       </c>
@@ -7570,7 +7591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>194</v>
       </c>
@@ -7587,7 +7608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>195</v>
       </c>
@@ -7604,7 +7625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
         <v>196</v>
       </c>
@@ -7621,7 +7642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>197</v>
       </c>
@@ -7638,7 +7659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>198</v>
       </c>
@@ -7655,7 +7676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>199</v>
       </c>
@@ -7672,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>200</v>
       </c>
@@ -7689,7 +7710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>201</v>
       </c>
@@ -7706,7 +7727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>202</v>
       </c>
@@ -7723,7 +7744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>203</v>
       </c>
@@ -7740,7 +7761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>204</v>
       </c>
@@ -7757,7 +7778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>205</v>
       </c>
@@ -7774,7 +7795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>206</v>
       </c>
@@ -7791,7 +7812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>207</v>
       </c>
@@ -7808,7 +7829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>208</v>
       </c>
@@ -7825,7 +7846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>209</v>
       </c>
@@ -7842,7 +7863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>210</v>
       </c>
@@ -7859,7 +7880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>211</v>
       </c>
@@ -7876,7 +7897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>212</v>
       </c>
@@ -7893,7 +7914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>213</v>
       </c>
@@ -7910,7 +7931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>214</v>
       </c>
@@ -7927,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>215</v>
       </c>
@@ -7944,7 +7965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
         <v>216</v>
       </c>
@@ -7961,7 +7982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>217</v>
       </c>
@@ -7978,7 +7999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
         <v>218</v>
       </c>
@@ -7995,7 +8016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>219</v>
       </c>
@@ -8012,7 +8033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
         <v>220</v>
       </c>
@@ -8029,7 +8050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
bug fixes + NA drop fix
</commit_message>
<xml_diff>
--- a/SWiMS_Codebook_v5.xlsx
+++ b/SWiMS_Codebook_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/telmer/switchdrive/Other Stuff/Actionuni/SWiMS/SWiMS_analyses/SWiMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkovacevic\Desktop\Ehrenamt\Actionuni\SWiMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2DFD4-22F5-7A44-98B9-C276D0624B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE76117B-00C5-4008-9F86-3056DC5BBDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="564">
   <si>
     <t>Nr</t>
   </si>
@@ -1567,18 +1567,12 @@
     <t>distribution</t>
   </si>
   <si>
-    <t>supervisor</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
     <t>workgroup</t>
   </si>
   <si>
-    <t>qrp</t>
-  </si>
-  <si>
     <t>qrp_pressure</t>
   </si>
   <si>
@@ -1603,9 +1597,6 @@
     <t>qrp_pressure_mh</t>
   </si>
   <si>
-    <t>stress_system</t>
-  </si>
-  <si>
     <t>stress_supervisor</t>
   </si>
   <si>
@@ -1633,9 +1624,6 @@
     <t>from DASS scale</t>
   </si>
   <si>
-    <t>facet_wrap with items above</t>
-  </si>
-  <si>
     <t>burnout</t>
   </si>
   <si>
@@ -1703,13 +1691,46 @@
   </si>
   <si>
     <t>Researcher aiming for a PhD//Postdoctoral researcher//Other researchers with a PhD//Other</t>
+  </si>
+  <si>
+    <t>stress_system2</t>
+  </si>
+  <si>
+    <t>stress_system3</t>
+  </si>
+  <si>
+    <t>stress_system1</t>
+  </si>
+  <si>
+    <t>supervisor1</t>
+  </si>
+  <si>
+    <t>supervisor2</t>
+  </si>
+  <si>
+    <t>supervisor3</t>
+  </si>
+  <si>
+    <t>institution1</t>
+  </si>
+  <si>
+    <t>institution2</t>
+  </si>
+  <si>
+    <t>qrp1</t>
+  </si>
+  <si>
+    <t>qrp2</t>
+  </si>
+  <si>
+    <t>qrp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1721,6 +1742,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2064,29 +2091,29 @@
   <dimension ref="A1:N232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E104" sqref="E104"/>
+      <selection pane="bottomRight" activeCell="N126" sqref="N126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.85546875" style="2"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="52.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="48.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="18.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2"/>
+    <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2"/>
+    <col min="7" max="7" width="48.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="2"/>
     <col min="9" max="9" width="47" style="2" customWidth="1"/>
-    <col min="10" max="13" width="12.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="39.1640625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="2"/>
+    <col min="10" max="13" width="12.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="39.140625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2115,22 +2142,22 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2141,7 +2168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2155,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2169,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2183,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2197,7 +2224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2211,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2225,7 +2252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2239,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2253,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2267,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2281,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2295,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2321,7 +2348,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2344,7 +2371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2367,7 +2394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2399,7 +2426,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2416,7 +2443,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2448,7 +2475,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18.5</v>
       </c>
@@ -2456,22 +2483,22 @@
         <v>225</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2497,7 +2524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2523,7 +2550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2549,7 +2576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2575,18 +2602,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22.5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>234</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>509</v>
@@ -2595,13 +2622,13 @@
         <v>510</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2633,27 +2660,27 @@
         <v>510</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23.5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2685,24 +2712,24 @@
         <v>510</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>24.5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>25</v>
       </c>
@@ -2728,7 +2755,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>26</v>
       </c>
@@ -2754,7 +2781,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>27</v>
       </c>
@@ -2768,7 +2795,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>28</v>
       </c>
@@ -2794,7 +2821,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>29</v>
       </c>
@@ -2826,27 +2853,27 @@
         <v>510</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>29.5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I35" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>30</v>
       </c>
@@ -2878,24 +2905,27 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>30.5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>534</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>31</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>32</v>
       </c>
@@ -2944,7 +2974,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>33</v>
       </c>
@@ -2976,7 +3006,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>34</v>
       </c>
@@ -3002,7 +3032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>35</v>
       </c>
@@ -3022,7 +3052,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>36</v>
       </c>
@@ -3042,7 +3072,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>37</v>
       </c>
@@ -3074,7 +3104,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>38</v>
       </c>
@@ -3100,7 +3130,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>39</v>
       </c>
@@ -3126,7 +3156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>40</v>
       </c>
@@ -3152,7 +3182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>41</v>
       </c>
@@ -3178,27 +3208,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>41.5</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>509</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>42</v>
       </c>
@@ -3224,7 +3254,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43</v>
       </c>
@@ -3250,7 +3280,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44</v>
       </c>
@@ -3276,7 +3306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45</v>
       </c>
@@ -3302,7 +3332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>46</v>
       </c>
@@ -3328,7 +3358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -3354,7 +3384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>48</v>
       </c>
@@ -3380,7 +3410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>49</v>
       </c>
@@ -3406,7 +3436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>50</v>
       </c>
@@ -3432,7 +3462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>51</v>
       </c>
@@ -3449,7 +3479,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>52</v>
       </c>
@@ -3475,13 +3505,13 @@
         <v>154</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>53</v>
       </c>
@@ -3507,13 +3537,13 @@
         <v>158</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>54</v>
       </c>
@@ -3539,13 +3569,13 @@
         <v>158</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>55</v>
       </c>
@@ -3571,13 +3601,13 @@
         <v>158</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>56</v>
       </c>
@@ -3603,13 +3633,13 @@
         <v>158</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>57</v>
       </c>
@@ -3635,13 +3665,13 @@
         <v>158</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>58</v>
       </c>
@@ -3667,13 +3697,13 @@
         <v>158</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>511</v>
+        <v>557</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>59</v>
       </c>
@@ -3699,13 +3729,13 @@
         <v>158</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>511</v>
+        <v>558</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>60</v>
       </c>
@@ -3731,13 +3761,13 @@
         <v>158</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>511</v>
+        <v>558</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>61</v>
       </c>
@@ -3763,13 +3793,13 @@
         <v>158</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>511</v>
+        <v>558</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>62</v>
       </c>
@@ -3795,13 +3825,13 @@
         <v>158</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>32</v>
+        <v>559</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>63</v>
       </c>
@@ -3827,13 +3857,13 @@
         <v>158</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>32</v>
+        <v>559</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>64</v>
       </c>
@@ -3859,13 +3889,13 @@
         <v>158</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>32</v>
+        <v>559</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>65</v>
       </c>
@@ -3891,13 +3921,13 @@
         <v>158</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>32</v>
+        <v>559</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>66</v>
       </c>
@@ -3923,13 +3953,13 @@
         <v>158</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>32</v>
+        <v>560</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>67</v>
       </c>
@@ -3955,13 +3985,13 @@
         <v>158</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>32</v>
+        <v>560</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>68</v>
       </c>
@@ -3987,13 +4017,13 @@
         <v>158</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>32</v>
+        <v>560</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>69</v>
       </c>
@@ -4019,7 +4049,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>70</v>
       </c>
@@ -4045,13 +4075,13 @@
         <v>158</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>71</v>
       </c>
@@ -4077,13 +4107,13 @@
         <v>158</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>72</v>
       </c>
@@ -4109,13 +4139,13 @@
         <v>158</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>73</v>
       </c>
@@ -4144,10 +4174,10 @@
         <v>201</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>74</v>
       </c>
@@ -4176,10 +4206,10 @@
         <v>201</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>75</v>
       </c>
@@ -4208,10 +4238,10 @@
         <v>201</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>76</v>
       </c>
@@ -4240,10 +4270,10 @@
         <v>201</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>77</v>
       </c>
@@ -4272,10 +4302,10 @@
         <v>201</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>78</v>
       </c>
@@ -4304,10 +4334,10 @@
         <v>201</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>79</v>
       </c>
@@ -4336,10 +4366,10 @@
         <v>201</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>80</v>
       </c>
@@ -4368,10 +4398,10 @@
         <v>201</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>81</v>
       </c>
@@ -4403,7 +4433,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>82</v>
       </c>
@@ -4429,13 +4459,13 @@
         <v>27</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>83</v>
       </c>
@@ -4461,13 +4491,13 @@
         <v>27</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>84</v>
       </c>
@@ -4493,13 +4523,13 @@
         <v>27</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>85</v>
       </c>
@@ -4525,13 +4555,13 @@
         <v>27</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>86</v>
       </c>
@@ -4557,13 +4587,13 @@
         <v>27</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>87</v>
       </c>
@@ -4589,13 +4619,13 @@
         <v>27</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>88</v>
       </c>
@@ -4621,13 +4651,13 @@
         <v>27</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>89</v>
       </c>
@@ -4653,13 +4683,13 @@
         <v>27</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>90</v>
       </c>
@@ -4685,13 +4715,13 @@
         <v>27</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>91</v>
       </c>
@@ -4717,13 +4747,13 @@
         <v>27</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>92</v>
       </c>
@@ -4749,13 +4779,13 @@
         <v>27</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>93</v>
       </c>
@@ -4781,13 +4811,13 @@
         <v>27</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>94</v>
       </c>
@@ -4813,13 +4843,13 @@
         <v>27</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>95</v>
       </c>
@@ -4845,13 +4875,13 @@
         <v>27</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>96</v>
       </c>
@@ -4877,13 +4907,13 @@
         <v>256</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>97</v>
       </c>
@@ -4909,13 +4939,13 @@
         <v>27</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>98</v>
       </c>
@@ -4941,7 +4971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>99</v>
       </c>
@@ -4967,7 +4997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>100</v>
       </c>
@@ -4993,7 +5023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>101</v>
       </c>
@@ -5019,7 +5049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>102</v>
       </c>
@@ -5045,7 +5075,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>103</v>
       </c>
@@ -5071,7 +5101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>104</v>
       </c>
@@ -5097,7 +5127,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>105</v>
       </c>
@@ -5123,13 +5153,13 @@
         <v>274</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>106</v>
       </c>
@@ -5155,13 +5185,13 @@
         <v>274</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>107</v>
       </c>
@@ -5187,13 +5217,13 @@
         <v>274</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>108</v>
       </c>
@@ -5219,13 +5249,13 @@
         <v>274</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>109</v>
       </c>
@@ -5251,13 +5281,13 @@
         <v>274</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>514</v>
+        <v>561</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>110</v>
       </c>
@@ -5283,13 +5313,13 @@
         <v>274</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>111</v>
       </c>
@@ -5315,13 +5345,13 @@
         <v>274</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>112</v>
       </c>
@@ -5347,13 +5377,13 @@
         <v>274</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>113</v>
       </c>
@@ -5379,13 +5409,13 @@
         <v>274</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>114</v>
       </c>
@@ -5411,13 +5441,13 @@
         <v>274</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>514</v>
+        <v>562</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>115</v>
       </c>
@@ -5443,13 +5473,13 @@
         <v>274</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>514</v>
+        <v>563</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>116</v>
       </c>
@@ -5475,13 +5505,13 @@
         <v>274</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>514</v>
+        <v>563</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>117</v>
       </c>
@@ -5507,13 +5537,13 @@
         <v>274</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>514</v>
+        <v>563</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>118</v>
       </c>
@@ -5539,13 +5569,13 @@
         <v>27</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>119</v>
       </c>
@@ -5571,13 +5601,13 @@
         <v>27</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>120</v>
       </c>
@@ -5603,13 +5633,13 @@
         <v>27</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>121</v>
       </c>
@@ -5635,13 +5665,13 @@
         <v>27</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>122</v>
       </c>
@@ -5667,13 +5697,13 @@
         <v>27</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>123</v>
       </c>
@@ -5699,13 +5729,13 @@
         <v>27</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>124</v>
       </c>
@@ -5731,13 +5761,13 @@
         <v>27</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>125</v>
       </c>
@@ -5763,13 +5793,13 @@
         <v>27</v>
       </c>
       <c r="J133" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K133" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>126</v>
       </c>
@@ -5795,13 +5825,13 @@
         <v>27</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K134" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>127</v>
       </c>
@@ -5827,13 +5857,13 @@
         <v>27</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>128</v>
       </c>
@@ -5847,7 +5877,7 @@
         <v>38</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>301</v>
@@ -5859,13 +5889,13 @@
         <v>320</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>129</v>
       </c>
@@ -5891,13 +5921,13 @@
         <v>27</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>130</v>
       </c>
@@ -5923,13 +5953,13 @@
         <v>327</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="K138" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>131</v>
       </c>
@@ -5961,7 +5991,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>132</v>
       </c>
@@ -5987,16 +6017,16 @@
         <v>335</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>523</v>
+        <v>555</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>133</v>
       </c>
@@ -6022,13 +6052,13 @@
         <v>335</v>
       </c>
       <c r="J141" s="2" t="s">
-        <v>523</v>
+        <v>555</v>
       </c>
       <c r="K141" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>134</v>
       </c>
@@ -6054,13 +6084,13 @@
         <v>335</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="K142" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>135</v>
       </c>
@@ -6086,13 +6116,13 @@
         <v>335</v>
       </c>
       <c r="J143" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>136</v>
       </c>
@@ -6118,13 +6148,13 @@
         <v>335</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="K144" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>137</v>
       </c>
@@ -6150,13 +6180,13 @@
         <v>335</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>523</v>
+        <v>553</v>
       </c>
       <c r="K145" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>138</v>
       </c>
@@ -6182,13 +6212,13 @@
         <v>335</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="K146" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>139</v>
       </c>
@@ -6214,13 +6244,13 @@
         <v>335</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="K147" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>140</v>
       </c>
@@ -6246,13 +6276,13 @@
         <v>335</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>141</v>
       </c>
@@ -6278,13 +6308,13 @@
         <v>335</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="K149" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>142</v>
       </c>
@@ -6310,13 +6340,13 @@
         <v>335</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K150" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>143</v>
       </c>
@@ -6342,13 +6372,13 @@
         <v>335</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>144</v>
       </c>
@@ -6374,13 +6404,13 @@
         <v>335</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>145</v>
       </c>
@@ -6406,13 +6436,13 @@
         <v>335</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>146</v>
       </c>
@@ -6438,13 +6468,13 @@
         <v>335</v>
       </c>
       <c r="J154" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="K154" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>147</v>
       </c>
@@ -6470,13 +6500,13 @@
         <v>335</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>148</v>
       </c>
@@ -6502,13 +6532,13 @@
         <v>335</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="K156" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>149</v>
       </c>
@@ -6534,13 +6564,13 @@
         <v>335</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="K157" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>150</v>
       </c>
@@ -6566,13 +6596,13 @@
         <v>335</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K158" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>151</v>
       </c>
@@ -6598,13 +6628,13 @@
         <v>335</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K159" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>152</v>
       </c>
@@ -6630,13 +6660,13 @@
         <v>335</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K160" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>153</v>
       </c>
@@ -6662,13 +6692,13 @@
         <v>335</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K161" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>154</v>
       </c>
@@ -6694,13 +6724,13 @@
         <v>335</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>155</v>
       </c>
@@ -6726,13 +6756,13 @@
         <v>335</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>156</v>
       </c>
@@ -6758,7 +6788,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>157</v>
       </c>
@@ -6778,7 +6808,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>158</v>
       </c>
@@ -6804,13 +6834,13 @@
         <v>388</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>159</v>
       </c>
@@ -6836,16 +6866,16 @@
         <v>392</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N167" s="2" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>160</v>
       </c>
@@ -6871,13 +6901,16 @@
         <v>392</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>161</v>
       </c>
@@ -6903,13 +6936,16 @@
         <v>392</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K169" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N169" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>162</v>
       </c>
@@ -6935,13 +6971,16 @@
         <v>392</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>163</v>
       </c>
@@ -6967,13 +7006,16 @@
         <v>392</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K171" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>164</v>
       </c>
@@ -6999,13 +7041,16 @@
         <v>392</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N172" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>165</v>
       </c>
@@ -7031,47 +7076,41 @@
         <v>392</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K173" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+      <c r="N173" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>165.5</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="J174" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="K174" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="N174" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>165.6</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>166</v>
       </c>
@@ -7097,18 +7136,18 @@
         <v>408</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>166.5</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>405</v>
@@ -7129,13 +7168,13 @@
         <v>408</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K177" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>167</v>
       </c>
@@ -7167,7 +7206,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>168</v>
       </c>
@@ -7193,13 +7232,13 @@
         <v>417</v>
       </c>
       <c r="J179" s="2" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="K179" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>169</v>
       </c>
@@ -7225,13 +7264,13 @@
         <v>417</v>
       </c>
       <c r="J180" s="2" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="K180" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>170</v>
       </c>
@@ -7257,7 +7296,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>171</v>
       </c>
@@ -7283,7 +7322,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>172</v>
       </c>
@@ -7297,7 +7336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>173</v>
       </c>
@@ -7311,7 +7350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>174</v>
       </c>
@@ -7325,7 +7364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>175</v>
       </c>
@@ -7339,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>176</v>
       </c>
@@ -7353,7 +7392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>177</v>
       </c>
@@ -7367,7 +7406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>178</v>
       </c>
@@ -7381,7 +7420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>179</v>
       </c>
@@ -7395,7 +7434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>180</v>
       </c>
@@ -7409,7 +7448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>181</v>
       </c>
@@ -7423,7 +7462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>182</v>
       </c>
@@ -7437,7 +7476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>183</v>
       </c>
@@ -7451,7 +7490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>184</v>
       </c>
@@ -7465,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>185</v>
       </c>
@@ -7479,7 +7518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>186</v>
       </c>
@@ -7493,7 +7532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>187</v>
       </c>
@@ -7507,7 +7546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>188</v>
       </c>
@@ -7518,7 +7557,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>189</v>
       </c>
@@ -7529,7 +7568,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>190</v>
       </c>
@@ -7543,7 +7582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>191</v>
       </c>
@@ -7560,7 +7599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>192</v>
       </c>
@@ -7577,7 +7616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>193</v>
       </c>
@@ -7594,7 +7633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>194</v>
       </c>
@@ -7611,7 +7650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>195</v>
       </c>
@@ -7628,7 +7667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>196</v>
       </c>
@@ -7645,7 +7684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>197</v>
       </c>
@@ -7662,7 +7701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>198</v>
       </c>
@@ -7679,7 +7718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>199</v>
       </c>
@@ -7696,7 +7735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>200</v>
       </c>
@@ -7713,7 +7752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>201</v>
       </c>
@@ -7730,7 +7769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>202</v>
       </c>
@@ -7747,7 +7786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>203</v>
       </c>
@@ -7764,7 +7803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>204</v>
       </c>
@@ -7781,7 +7820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>205</v>
       </c>
@@ -7798,7 +7837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>206</v>
       </c>
@@ -7815,7 +7854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>207</v>
       </c>
@@ -7832,7 +7871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>208</v>
       </c>
@@ -7849,7 +7888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>209</v>
       </c>
@@ -7866,7 +7905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>210</v>
       </c>
@@ -7883,7 +7922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>211</v>
       </c>
@@ -7900,7 +7939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>212</v>
       </c>
@@ -7917,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>213</v>
       </c>
@@ -7934,7 +7973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>214</v>
       </c>
@@ -7951,7 +7990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>215</v>
       </c>
@@ -7968,7 +8007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>216</v>
       </c>
@@ -7985,7 +8024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>217</v>
       </c>
@@ -8002,7 +8041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>218</v>
       </c>
@@ -8019,7 +8058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>219</v>
       </c>
@@ -8036,7 +8075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>220</v>
       </c>
@@ -8053,7 +8092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>221</v>
       </c>
@@ -8071,6 +8110,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L1:M25 L27:M27 L28 L29:M33 L35:M35 L36 L37:M1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>

</xml_diff>